<commit_message>
updates with yac and drops for active and rookies
</commit_message>
<xml_diff>
--- a/data/rookies.xlsx
+++ b/data/rookies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victornorris/Code/projects/DraftPredictor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967E9639-0DCB-654C-8723-06B3A3458680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A4F36D-96F0-0540-ABEC-8DDB00425A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-3640" windowWidth="24060" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -146,9 +146,6 @@
     <t>Brenden Rice</t>
   </si>
   <si>
-    <t>Rick Pearsall</t>
-  </si>
-  <si>
     <t>6'1</t>
   </si>
   <si>
@@ -201,13 +198,46 @@
   </si>
   <si>
     <t>6'5</t>
+  </si>
+  <si>
+    <t>Javon Baker</t>
+  </si>
+  <si>
+    <t>Jalen Coker</t>
+  </si>
+  <si>
+    <t>Jacob Cowing</t>
+  </si>
+  <si>
+    <t>Cornelius Johnson</t>
+  </si>
+  <si>
+    <t>Luke McCaffrey</t>
+  </si>
+  <si>
+    <t>Tayvion Robinson</t>
+  </si>
+  <si>
+    <t>TeamRanking</t>
+  </si>
+  <si>
+    <t>Drops</t>
+  </si>
+  <si>
+    <t>Yac</t>
+  </si>
+  <si>
+    <t>drp%</t>
+  </si>
+  <si>
+    <t>Ricky Pearsall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +255,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Proxima Nova"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF3F05E0"/>
+      <name val="Proxima Nova"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -268,17 +318,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,21 +636,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
     <col min="9" max="9" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="18" width="9" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="9" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="11.33203125" customWidth="1"/>
+    <col min="21" max="22" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,22 +710,34 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -698,23 +775,36 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <f>R2/(R2+F2)</f>
+        <v>6.0606060606060608E-2</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>787</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U27" ca="1" si="0">YEAR(TODAY())-B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <f t="shared" ref="Y2:Y33" ca="1" si="0">YEAR(TODAY())-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -752,23 +842,36 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <f>R3/(R3+F3)</f>
+        <v>7.3529411764705885E-2</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1252</v>
       </c>
       <c r="U3">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -806,25 +909,38 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <f t="shared" ref="S4:S33" si="1">R4/(R4+F4)</f>
+        <v>6.5502183406113537E-2</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1119</v>
       </c>
       <c r="U4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>2024</v>
@@ -833,7 +949,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5">
         <v>198</v>
@@ -860,23 +976,36 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.285714285714286E-2</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="U5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -914,23 +1043,36 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.0459770114942528E-2</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>875</v>
       </c>
       <c r="U6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -968,23 +1110,36 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>7.7519379844961239E-2</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>783</v>
       </c>
       <c r="U7">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1022,23 +1177,36 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.771929824561403E-2</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>430</v>
       </c>
       <c r="U8">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1076,23 +1244,36 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>573</v>
       </c>
       <c r="U9">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1130,23 +1311,36 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>275</v>
       </c>
       <c r="U10">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1184,23 +1378,36 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>6.6115702479338845E-2</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>604</v>
       </c>
       <c r="U11">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1238,23 +1445,36 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>543</v>
       </c>
       <c r="U12">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1292,23 +1512,36 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>7.0754716981132074E-2</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>1421</v>
       </c>
       <c r="U13">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1346,23 +1579,36 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5.2980132450331126E-2</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="U14">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1400,25 +1646,38 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.2644628099173556E-2</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>711</v>
       </c>
       <c r="U15">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B16">
         <v>2024</v>
@@ -1427,7 +1686,7 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16">
         <v>192</v>
@@ -1454,25 +1713,38 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>3.6363636363636362E-2</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>878</v>
       </c>
       <c r="U16">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17">
         <v>2024</v>
@@ -1481,7 +1753,7 @@
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17">
         <v>192</v>
@@ -1508,25 +1780,38 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>7.8651685393258425E-2</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>925</v>
       </c>
       <c r="U17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18">
         <v>2024</v>
@@ -1535,7 +1820,7 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <v>237</v>
@@ -1562,25 +1847,38 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R18">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.12820512820512819</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>541</v>
       </c>
       <c r="U18">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>2024</v>
@@ -1616,25 +1914,38 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>6.1403508771929821E-2</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>576</v>
       </c>
       <c r="U19">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20">
         <v>2024</v>
@@ -1670,25 +1981,38 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.13675213675213677</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>486</v>
       </c>
       <c r="U20">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>2024</v>
@@ -1697,7 +2021,7 @@
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21">
         <v>185</v>
@@ -1724,25 +2048,38 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.2391304347826081E-2</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>1057</v>
       </c>
       <c r="U21">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <v>2024</v>
@@ -1751,7 +2088,7 @@
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22">
         <v>210</v>
@@ -1778,25 +2115,38 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R22">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="S22">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>4.779411764705882E-2</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>2117</v>
       </c>
       <c r="U22">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <v>2024</v>
@@ -1805,7 +2155,7 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23">
         <v>200</v>
@@ -1832,25 +2182,38 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R23">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S23">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>8.1632653061224483E-2</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>1068</v>
       </c>
       <c r="U23">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24">
         <v>2024</v>
@@ -1859,7 +2222,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24">
         <v>205</v>
@@ -1886,25 +2249,38 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>7.407407407407407E-2</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>399</v>
       </c>
       <c r="U24">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25">
         <v>2024</v>
@@ -1940,31 +2316,47 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S25">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="T25">
-        <v>0</v>
+        <v>449</v>
       </c>
       <c r="U25">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>2024</v>
+      </c>
+      <c r="C26">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
         <v>51</v>
-      </c>
-      <c r="B26">
-        <v>2024</v>
-      </c>
-      <c r="D26" t="s">
-        <v>52</v>
       </c>
       <c r="E26">
         <v>194</v>
@@ -1991,52 +2383,65 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S26">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5423728813559324E-2</v>
       </c>
       <c r="T26">
-        <v>0</v>
+        <v>1353</v>
       </c>
       <c r="U26">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B27">
         <v>2024</v>
       </c>
       <c r="C27">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27">
-        <v>185</v>
+        <v>208</v>
       </c>
       <c r="F27">
-        <v>266</v>
+        <v>117</v>
       </c>
       <c r="G27">
-        <v>3386</v>
+        <v>2051</v>
       </c>
       <c r="H27">
-        <v>12.7</v>
+        <v>17.5</v>
       </c>
       <c r="I27">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="J27">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -2045,21 +2450,509 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S27">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.11363636363636363</v>
       </c>
       <c r="T27">
-        <v>0</v>
+        <v>651</v>
       </c>
       <c r="U27">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28">
+        <v>2024</v>
+      </c>
+      <c r="C28">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28">
+        <v>213</v>
+      </c>
+      <c r="F28">
+        <v>164</v>
+      </c>
+      <c r="G28">
+        <v>2715</v>
+      </c>
+      <c r="H28">
+        <f>G28/F28</f>
+        <v>16.554878048780488</v>
+      </c>
+      <c r="I28">
+        <v>31</v>
+      </c>
+      <c r="J28">
+        <v>39</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28">
+        <v>40</v>
+      </c>
+      <c r="R28">
+        <v>13</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="1"/>
+        <v>7.3446327683615822E-2</v>
+      </c>
+      <c r="T28">
+        <v>835</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29">
+        <v>2024</v>
+      </c>
+      <c r="C29">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29">
+        <v>170</v>
+      </c>
+      <c r="F29">
+        <v>316</v>
+      </c>
+      <c r="G29">
+        <v>4477</v>
+      </c>
+      <c r="H29">
+        <v>14.2</v>
+      </c>
+      <c r="I29">
+        <v>33</v>
+      </c>
+      <c r="J29">
+        <v>58</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29">
+        <v>11</v>
+      </c>
+      <c r="R29">
+        <v>33</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="1"/>
+        <v>9.4555873925501438E-2</v>
+      </c>
+      <c r="T29">
+        <v>1992</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30">
+        <v>2024</v>
+      </c>
+      <c r="C30">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30">
+        <v>211</v>
+      </c>
+      <c r="F30">
+        <v>138</v>
+      </c>
+      <c r="G30">
+        <v>2038</v>
+      </c>
+      <c r="H30">
+        <v>14.8</v>
+      </c>
+      <c r="I30">
+        <v>14</v>
+      </c>
+      <c r="J30">
+        <v>61</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>17</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="1"/>
+        <v>0.10967741935483871</v>
+      </c>
+      <c r="T30">
+        <v>626</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31">
+        <v>2024</v>
+      </c>
+      <c r="C31">
+        <v>23</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31">
+        <v>200</v>
+      </c>
+      <c r="F31">
+        <v>131</v>
+      </c>
+      <c r="G31">
+        <v>1732</v>
+      </c>
+      <c r="H31">
+        <v>13.2</v>
+      </c>
+      <c r="I31">
+        <v>19</v>
+      </c>
+      <c r="J31">
+        <v>24</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31">
+        <v>40</v>
+      </c>
+      <c r="R31">
+        <v>8</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="1"/>
+        <v>5.7553956834532377E-2</v>
+      </c>
+      <c r="T31">
+        <v>707</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32">
+        <v>2024</v>
+      </c>
+      <c r="D32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32">
+        <v>187</v>
+      </c>
+      <c r="F32">
+        <v>194</v>
+      </c>
+      <c r="G32">
+        <v>2604</v>
+      </c>
+      <c r="H32">
+        <v>13.4</v>
+      </c>
+      <c r="I32">
+        <v>16</v>
+      </c>
+      <c r="J32">
+        <v>60</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32">
+        <v>40</v>
+      </c>
+      <c r="R32">
+        <v>13</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="1"/>
+        <v>6.280193236714976E-2</v>
+      </c>
+      <c r="T32">
+        <v>1348</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33">
+        <v>2024</v>
+      </c>
+      <c r="C33">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33">
+        <v>185</v>
+      </c>
+      <c r="F33">
+        <v>266</v>
+      </c>
+      <c r="G33">
+        <v>3386</v>
+      </c>
+      <c r="H33">
+        <v>12.7</v>
+      </c>
+      <c r="I33">
+        <v>38</v>
+      </c>
+      <c r="J33">
+        <v>50</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33">
+        <v>9</v>
+      </c>
+      <c r="R33">
+        <v>16</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="1"/>
+        <v>5.6737588652482268E-2</v>
+      </c>
+      <c r="T33">
+        <v>1325</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:25" ht="25" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:25" ht="25" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:25" ht="25" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="65" spans="1:1" ht="25" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+    </row>
+    <row r="66" spans="1:1" ht="25" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" spans="1:1" ht="25" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="4"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="4"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="4"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added combine stats for 2024 players
</commit_message>
<xml_diff>
--- a/data/rookies.xlsx
+++ b/data/rookies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victornorris/Code/projects/DraftPredictor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A4F36D-96F0-0540-ABEC-8DDB00425A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424281F4-0B9D-A04A-AAF2-A56B82E733FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -231,13 +231,16 @@
   </si>
   <si>
     <t>Ricky Pearsall</t>
+  </si>
+  <si>
+    <t>Tahj Washington</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +278,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -638,20 +647,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P37" sqref="P37"/>
+      <selection pane="bottomLeft" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" customWidth="1"/>
     <col min="9" max="9" width="3.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="16" width="9" customWidth="1"/>
@@ -902,12 +912,23 @@
       <c r="J4">
         <v>40</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="K4" s="2">
+        <v>4.45</v>
+      </c>
+      <c r="L4" s="2">
+        <v>39</v>
+      </c>
       <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="N4" s="2">
+        <f>10*12+4</f>
+        <v>124</v>
+      </c>
+      <c r="O4" s="2">
+        <v>6.88</v>
+      </c>
+      <c r="P4" s="2">
+        <v>4.03</v>
+      </c>
       <c r="Q4">
         <v>2</v>
       </c>
@@ -969,10 +990,18 @@
       <c r="J5">
         <v>38</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="K5" s="2">
+        <v>4.33</v>
+      </c>
+      <c r="L5" s="2">
+        <v>38.5</v>
+      </c>
+      <c r="M5" s="2">
+        <v>11</v>
+      </c>
+      <c r="N5" s="2">
+        <v>126</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5">
@@ -1036,12 +1065,23 @@
       <c r="J6">
         <v>40</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="K6" s="2">
+        <v>4.41</v>
+      </c>
+      <c r="L6" s="2">
+        <v>39</v>
+      </c>
       <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="N6" s="2">
+        <f>10*12+4</f>
+        <v>124</v>
+      </c>
+      <c r="O6" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="P6" s="2">
+        <v>4.3099999999999996</v>
+      </c>
       <c r="Q6">
         <v>6</v>
       </c>
@@ -1103,10 +1143,18 @@
       <c r="J7">
         <v>39</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="K7" s="2">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="L7" s="2">
+        <v>36</v>
+      </c>
+      <c r="M7" s="2">
+        <v>13</v>
+      </c>
+      <c r="N7" s="2">
+        <v>124</v>
+      </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7">
@@ -1170,10 +1218,17 @@
       <c r="J8">
         <v>28</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="K8" s="2">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="L8" s="2">
+        <v>40.5</v>
+      </c>
       <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2">
+        <f>11*12+2</f>
+        <v>134</v>
+      </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8">
@@ -1237,10 +1292,17 @@
       <c r="J9">
         <v>34</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="K9" s="2">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="L9" s="2">
+        <v>38</v>
+      </c>
       <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2">
+        <f>10*12+7</f>
+        <v>127</v>
+      </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9">
@@ -1304,10 +1366,17 @@
       <c r="J10">
         <v>35</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="K10" s="2">
+        <v>4.34</v>
+      </c>
+      <c r="L10" s="2">
+        <v>39.5</v>
+      </c>
       <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="N10" s="2">
+        <f>11*12+4</f>
+        <v>136</v>
+      </c>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10">
@@ -1371,10 +1440,16 @@
       <c r="J11">
         <v>53</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="K11" s="2">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="L11" s="2">
+        <v>40.5</v>
+      </c>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="N11" s="2">
+        <v>126</v>
+      </c>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11">
@@ -1438,10 +1513,17 @@
       <c r="J12">
         <v>50</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="K12" s="2">
+        <v>4.45</v>
+      </c>
+      <c r="L12" s="2">
+        <v>38.5</v>
+      </c>
       <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="N12" s="2">
+        <f>11*12+1</f>
+        <v>133</v>
+      </c>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12">
@@ -1505,10 +1587,17 @@
       <c r="J13">
         <v>39</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="K13" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="L13" s="2">
+        <v>41</v>
+      </c>
       <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2">
+        <f>10*12+11</f>
+        <v>131</v>
+      </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13">
@@ -1572,10 +1661,17 @@
       <c r="J14">
         <v>41</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="K14" s="2">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="L14" s="2">
+        <v>37.5</v>
+      </c>
       <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2">
+        <f>10*12+9</f>
+        <v>129</v>
+      </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14">
@@ -1639,10 +1735,18 @@
       <c r="J15">
         <v>43</v>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="K15" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="L15" s="2">
+        <v>36.5</v>
+      </c>
+      <c r="M15" s="2">
+        <v>13</v>
+      </c>
+      <c r="N15" s="2">
+        <v>119</v>
+      </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15">
@@ -1706,12 +1810,25 @@
       <c r="J16">
         <v>55</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="K16" s="2">
+        <v>4.41</v>
+      </c>
+      <c r="L16" s="2">
+        <v>42</v>
+      </c>
+      <c r="M16" s="2">
+        <v>17</v>
+      </c>
+      <c r="N16" s="2">
+        <f>10*12+9</f>
+        <v>129</v>
+      </c>
+      <c r="O16" s="2">
+        <v>6.64</v>
+      </c>
+      <c r="P16" s="2">
+        <v>4.05</v>
+      </c>
       <c r="Q16">
         <v>40</v>
       </c>
@@ -1773,12 +1890,23 @@
       <c r="J17">
         <v>38</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="K17" s="2">
+        <v>4.47</v>
+      </c>
+      <c r="L17" s="2">
+        <v>37</v>
+      </c>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="N17" s="2">
+        <f>10*12+7</f>
+        <v>127</v>
+      </c>
+      <c r="O17" s="2">
+        <v>6.94</v>
+      </c>
+      <c r="P17" s="2">
+        <v>4.18</v>
+      </c>
       <c r="Q17">
         <v>2</v>
       </c>
@@ -1840,12 +1968,21 @@
       <c r="J18">
         <v>32</v>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="K18" s="2">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="L18" s="2">
+        <v>37</v>
+      </c>
       <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+      <c r="N18" s="2">
+        <f>10*12+8</f>
+        <v>128</v>
+      </c>
       <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
+      <c r="P18" s="2">
+        <v>4.1100000000000003</v>
+      </c>
       <c r="Q18">
         <v>6</v>
       </c>
@@ -1907,9 +2044,13 @@
       <c r="J19">
         <v>36</v>
       </c>
-      <c r="K19" s="2"/>
+      <c r="K19" s="2">
+        <v>4.3899999999999997</v>
+      </c>
       <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
+      <c r="M19" s="2">
+        <v>12</v>
+      </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -2041,11 +2182,19 @@
       <c r="J21">
         <v>49</v>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="K21" s="2">
+        <v>4.46</v>
+      </c>
+      <c r="L21" s="2">
+        <v>34</v>
+      </c>
       <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
+      <c r="N21" s="2">
+        <v>120</v>
+      </c>
+      <c r="O21" s="2">
+        <v>7.16</v>
+      </c>
       <c r="P21" s="2"/>
       <c r="Q21">
         <v>19</v>
@@ -2177,7 +2326,9 @@
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
+      <c r="M23" s="2">
+        <v>21</v>
+      </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -2376,10 +2527,19 @@
       <c r="J26">
         <v>52</v>
       </c>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="K26" s="2">
+        <v>4.47</v>
+      </c>
+      <c r="L26" s="2">
+        <v>42.5</v>
+      </c>
+      <c r="M26" s="2">
+        <v>19</v>
+      </c>
+      <c r="N26" s="2">
+        <f>10*12+6</f>
+        <v>126</v>
+      </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26">
@@ -2443,10 +2603,16 @@
       <c r="J27">
         <v>46</v>
       </c>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
+      <c r="K27" s="2">
+        <v>4.54</v>
+      </c>
+      <c r="L27" s="2">
+        <v>37</v>
+      </c>
       <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
+      <c r="N27" s="2">
+        <v>121</v>
+      </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27">
@@ -2511,10 +2677,16 @@
       <c r="J28">
         <v>39</v>
       </c>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
+      <c r="K28" s="2">
+        <v>4.57</v>
+      </c>
+      <c r="L28" s="2">
+        <v>42.5</v>
+      </c>
       <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="N28" s="2">
+        <v>128</v>
+      </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28">
@@ -2578,12 +2750,23 @@
       <c r="J29">
         <v>58</v>
       </c>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="K29" s="2">
+        <v>4.38</v>
+      </c>
+      <c r="L29" s="2">
+        <v>36</v>
+      </c>
       <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
+      <c r="N29" s="2">
+        <f>9*12+11</f>
+        <v>119</v>
+      </c>
+      <c r="O29" s="2">
+        <v>7.02</v>
+      </c>
+      <c r="P29" s="2">
+        <v>4.32</v>
+      </c>
       <c r="Q29">
         <v>11</v>
       </c>
@@ -2645,10 +2828,17 @@
       <c r="J30">
         <v>61</v>
       </c>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
+      <c r="K30" s="2">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="L30" s="2">
+        <v>37.5</v>
+      </c>
       <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="N30" s="2">
+        <f>10*12+7</f>
+        <v>127</v>
+      </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30">
@@ -2712,12 +2902,22 @@
       <c r="J31">
         <v>24</v>
       </c>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
+      <c r="K31" s="2">
+        <v>4.46</v>
+      </c>
+      <c r="L31" s="2">
+        <v>36</v>
+      </c>
       <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
+      <c r="N31" s="2">
+        <v>121</v>
+      </c>
+      <c r="O31" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="P31" s="2">
+        <v>4.0199999999999996</v>
+      </c>
       <c r="Q31">
         <v>40</v>
       </c>
@@ -2879,6 +3079,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34">
+        <v>2024</v>
+      </c>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2">
+        <v>35</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2">
+        <f>10*12+2</f>
+        <v>122</v>
+      </c>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" ref="Y34" ca="1" si="2">YEAR(TODAY())-B34</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
     </row>
@@ -2955,6 +3190,7 @@
       <c r="A74" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>